<commit_message>
📊 Relatório Oficial Atualizado: Sun Feb 15 18:54:30 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_Oficial.xlsx
+++ b/Relatorio_Oficial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Data</t>
   </si>
@@ -28,6 +28,18 @@
     <t>Tipo</t>
   </si>
   <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Fator</t>
+  </si>
+  <si>
+    <t>% Banca</t>
+  </si>
+  <si>
+    <t>Investido ($)</t>
+  </si>
+  <si>
     <t>Entrada</t>
   </si>
   <si>
@@ -64,18 +76,27 @@
     <t>15/02/2026 10:55:12</t>
   </si>
   <si>
+    <t>15/02/2026 14:49:54</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
     <t>BTC-USD</t>
   </si>
   <si>
+    <t>ETH-USD</t>
+  </si>
+  <si>
     <t>Depósito</t>
   </si>
   <si>
     <t>GRID</t>
   </si>
   <si>
+    <t>SNIPER</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -85,10 +106,19 @@
     <t>BUY</t>
   </si>
   <si>
+    <t>1.0x</t>
+  </si>
+  <si>
+    <t>0.0%</t>
+  </si>
+  <si>
     <t>Trade Antigo</t>
   </si>
   <si>
     <t>ADX 20.3 | RSI 30.4 &lt; 45 (Oversold)</t>
+  </si>
+  <si>
+    <t>ADX 37.3 (Trend) | RSI 22.1 &lt; 28</t>
   </si>
   <si>
     <t>✅ TAKE PROFIT</t>
@@ -101,9 +131,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="$ #,##0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$ #,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -157,13 +186,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -201,24 +229,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Performance: Trades Realizados</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -237,14 +247,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Relatorio_Trades!$A$2:$A$5</c:f>
+              <c:f>Relatorio_Trades!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -257,15 +266,18 @@
                 <c:pt idx="3">
                   <c:v>15/02/2026 10:55:12</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>15/02/2026 14:49:54</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Relatorio_Trades!$L$2:$L$5</c:f>
+              <c:f>Relatorio_Trades!$P$2:$P$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -277,6 +289,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>60.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,24 +321,6 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Saldo ($)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010001"/>
@@ -349,16 +346,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -665,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -673,204 +670,315 @@
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="8" width="14.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11" max="12" width="18.7109375" style="3" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="12" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="P3">
+        <v>60.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>60</v>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>70331.96875</v>
+      </c>
+      <c r="J4" s="1">
+        <v>69474.2734375</v>
+      </c>
+      <c r="K4" s="1">
+        <v>69628.6490625</v>
+      </c>
+      <c r="L4" s="1">
+        <v>70894.62450000001</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="P4">
+        <v>60.17</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="5" spans="1:16">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>69456.625</v>
+      </c>
+      <c r="J5" s="1">
+        <v>68860.03125</v>
+      </c>
+      <c r="K5" s="1">
+        <v>70151.19125</v>
+      </c>
+      <c r="L5" s="1">
+        <v>68900.97199999999</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="2">
+        <v>-0.06</v>
+      </c>
+      <c r="P5">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0.08</v>
-      </c>
-      <c r="L3" s="3">
-        <v>60.08</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2">
-        <v>70331.96875</v>
-      </c>
-      <c r="F4" s="2">
-        <v>69474.2734375</v>
-      </c>
-      <c r="G4" s="2">
-        <v>69628.6490625</v>
-      </c>
-      <c r="H4" s="2">
-        <v>70894.62450000001</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0.09</v>
-      </c>
-      <c r="L4" s="3">
-        <v>60.17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2">
-        <v>69456.625</v>
-      </c>
-      <c r="F5" s="2">
-        <v>68860.03125</v>
-      </c>
-      <c r="G5" s="2">
-        <v>70151.19125</v>
-      </c>
-      <c r="H5" s="2">
-        <v>68900.97199999999</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="3">
-        <v>-0.06</v>
-      </c>
-      <c r="L5" s="3">
-        <v>60.1</v>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2002.409912109375</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1968.935913085938</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2052.470159912109</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1972.373763427734</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="2">
+        <v>-0.75</v>
+      </c>
+      <c r="P6">
+        <v>59.35</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K1000">
+  <conditionalFormatting sqref="N2:N1000">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
📊 Relatório Oficial Atualizado: Wed Feb 18 23:38:08 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_Oficial.xlsx
+++ b/Relatorio_Oficial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>Data</t>
   </si>
@@ -79,6 +79,54 @@
     <t>15/02/2026 14:49:54</t>
   </si>
   <si>
+    <t>15/02/2026 16:06:49</t>
+  </si>
+  <si>
+    <t>16/02/2026 10:54:52</t>
+  </si>
+  <si>
+    <t>16/02/2026 12:35:54</t>
+  </si>
+  <si>
+    <t>16/02/2026 15:24:50</t>
+  </si>
+  <si>
+    <t>16/02/2026 19:02:52</t>
+  </si>
+  <si>
+    <t>16/02/2026 21:52:54</t>
+  </si>
+  <si>
+    <t>17/02/2026 01:35:55</t>
+  </si>
+  <si>
+    <t>17/02/2026 07:54:53</t>
+  </si>
+  <si>
+    <t>17/02/2026 11:45:55</t>
+  </si>
+  <si>
+    <t>17/02/2026 13:08:51</t>
+  </si>
+  <si>
+    <t>17/02/2026 14:15:53</t>
+  </si>
+  <si>
+    <t>18/02/2026 03:29:58</t>
+  </si>
+  <si>
+    <t>18/02/2026 05:21:50</t>
+  </si>
+  <si>
+    <t>18/02/2026 08:10:52</t>
+  </si>
+  <si>
+    <t>18/02/2026 12:43:58</t>
+  </si>
+  <si>
+    <t>18/02/2026 16:39:53</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -88,6 +136,18 @@
     <t>ETH-USD</t>
   </si>
   <si>
+    <t>XRP-USD</t>
+  </si>
+  <si>
+    <t>SOL-USD</t>
+  </si>
+  <si>
+    <t>ADA-USD</t>
+  </si>
+  <si>
+    <t>BNB-USD</t>
+  </si>
+  <si>
     <t>Depósito</t>
   </si>
   <si>
@@ -109,9 +169,36 @@
     <t>1.0x</t>
   </si>
   <si>
+    <t>10.5x</t>
+  </si>
+  <si>
+    <t>4.0x</t>
+  </si>
+  <si>
+    <t>1.5x</t>
+  </si>
+  <si>
+    <t>2.5x</t>
+  </si>
+  <si>
     <t>0.0%</t>
   </si>
   <si>
+    <t>95.0%</t>
+  </si>
+  <si>
+    <t>16.0%</t>
+  </si>
+  <si>
+    <t>4.0%</t>
+  </si>
+  <si>
+    <t>6.0%</t>
+  </si>
+  <si>
+    <t>10.0%</t>
+  </si>
+  <si>
     <t>Trade Antigo</t>
   </si>
   <si>
@@ -119,6 +206,54 @@
   </si>
   <si>
     <t>ADX 37.3 (Trend) | RSI 22.1 &lt; 28</t>
+  </si>
+  <si>
+    <t>ADX 36.6 (Trend) | RSI 27.3 &lt; 28</t>
+  </si>
+  <si>
+    <t>ADX 36.4 | RSI 26.9 &lt; 28</t>
+  </si>
+  <si>
+    <t>ADX 18.6 | RSI 33.3 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 18.1 | RSI 29.1 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 9.3 | RSI 58.1 &gt; 55</t>
+  </si>
+  <si>
+    <t>ADX 17.3 | RSI 70.1 &gt; 55</t>
+  </si>
+  <si>
+    <t>ADX 22.0 | RSI 69.2 &gt; 55</t>
+  </si>
+  <si>
+    <t>ADX 21.7 | RSI 37.9 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 23.5 | RSI 30.3 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 21.4 | RSI 29.0 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 21.5 | RSI 60.6 &gt; 55</t>
+  </si>
+  <si>
+    <t>ADX 20.7 | RSI 43.9 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 10.6 | RSI 38.6 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 22.8 | RSI 70.9 &gt; 55</t>
+  </si>
+  <si>
+    <t>ADX 22.8 | RSI 30.9 &lt; 45</t>
+  </si>
+  <si>
+    <t>ADX 18.8 | RSI 32.8 &lt; 45</t>
   </si>
   <si>
     <t>✅ TAKE PROFIT</t>
@@ -251,9 +386,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Relatorio_Trades!$A$2:$A$6</c:f>
+              <c:f>Relatorio_Trades!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Inicio</c:v>
                 </c:pt>
@@ -268,16 +403,64 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15/02/2026 14:49:54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15/02/2026 16:06:49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16/02/2026 10:54:52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16/02/2026 12:35:54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16/02/2026 15:24:50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16/02/2026 19:02:52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16/02/2026 21:52:54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17/02/2026 01:35:55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17/02/2026 07:54:53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17/02/2026 11:45:55</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17/02/2026 13:08:51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17/02/2026 14:15:53</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18/02/2026 03:29:58</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18/02/2026 05:21:50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18/02/2026 08:10:52</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18/02/2026 12:43:58</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18/02/2026 16:39:53</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Relatorio_Trades!$P$2:$P$6</c:f>
+              <c:f>Relatorio_Trades!$P$2:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
                 </c:pt>
@@ -292,6 +475,54 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>59.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55.12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.06</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>55.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55.26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>55.33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>55.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55.48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55.57</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -732,22 +963,22 @@
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -765,10 +996,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -782,22 +1013,22 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -815,10 +1046,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="O3" s="2">
         <v>0.08</v>
@@ -832,22 +1063,22 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -865,10 +1096,10 @@
         <v>70894.62450000001</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="O4" s="2">
         <v>0.09</v>
@@ -882,22 +1113,22 @@
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
@@ -915,10 +1146,10 @@
         <v>68900.97199999999</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="O5" s="2">
         <v>-0.06</v>
@@ -932,22 +1163,22 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
@@ -965,16 +1196,816 @@
         <v>1972.373763427734</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="O6" s="2">
         <v>-0.75</v>
       </c>
       <c r="P6">
         <v>59.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="2">
+        <v>32.64</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1.488950371742249</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.466265439987183</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.526174131035805</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1.466616116166115</v>
+      </c>
+      <c r="M7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="2">
+        <v>-1.49</v>
+      </c>
+      <c r="P7">
+        <v>57.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="2">
+        <v>54.97</v>
+      </c>
+      <c r="I8" s="1">
+        <v>85.61427307128906</v>
+      </c>
+      <c r="J8" s="1">
+        <v>84.25973510742188</v>
+      </c>
+      <c r="K8" s="1">
+        <v>87.75462989807129</v>
+      </c>
+      <c r="L8" s="1">
+        <v>84.33005897521973</v>
+      </c>
+      <c r="M8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" s="2">
+        <v>-2.61</v>
+      </c>
+      <c r="P8">
+        <v>55.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8.84</v>
+      </c>
+      <c r="I9" s="1">
+        <v>84.13960266113281</v>
+      </c>
+      <c r="J9" s="1">
+        <v>82.862548828125</v>
+      </c>
+      <c r="K9" s="1">
+        <v>84.98099868774415</v>
+      </c>
+      <c r="L9" s="1">
+        <v>83.46648583984376</v>
+      </c>
+      <c r="M9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="P9">
+        <v>54.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8.779999999999999</v>
+      </c>
+      <c r="I10" s="1">
+        <v>67483.3125</v>
+      </c>
+      <c r="J10" s="1">
+        <v>68177.53125</v>
+      </c>
+      <c r="K10" s="1">
+        <v>68158.145625</v>
+      </c>
+      <c r="L10" s="1">
+        <v>66943.446</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="P10">
+        <v>55.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2.2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.2841982543468475</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.2868249416351318</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.2813562718033791</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.2864718403816223</v>
+      </c>
+      <c r="M11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="2">
+        <v>-0.06</v>
+      </c>
+      <c r="P11">
+        <v>55.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>86.013427734375</v>
+      </c>
+      <c r="J12" s="1">
+        <v>86.7574462890625</v>
+      </c>
+      <c r="K12" s="1">
+        <v>85.15329345703125</v>
+      </c>
+      <c r="L12" s="1">
+        <v>86.70153515625</v>
+      </c>
+      <c r="M12" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" s="2">
+        <v>-0.08</v>
+      </c>
+      <c r="P12">
+        <v>54.97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>68989.796875</v>
+      </c>
+      <c r="J13" s="1">
+        <v>68267.84375</v>
+      </c>
+      <c r="K13" s="1">
+        <v>68299.89890625</v>
+      </c>
+      <c r="L13" s="1">
+        <v>69541.71524999999</v>
+      </c>
+      <c r="M13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="P13">
+        <v>55.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="I14" s="1">
+        <v>68276.8359375</v>
+      </c>
+      <c r="J14" s="1">
+        <v>67713.6875</v>
+      </c>
+      <c r="K14" s="1">
+        <v>68959.604296875</v>
+      </c>
+      <c r="L14" s="1">
+        <v>67730.62125</v>
+      </c>
+      <c r="M14" t="s">
+        <v>71</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="P14">
+        <v>55.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3.31</v>
+      </c>
+      <c r="I15" s="1">
+        <v>84.93430328369141</v>
+      </c>
+      <c r="J15" s="1">
+        <v>84.23800659179688</v>
+      </c>
+      <c r="K15" s="1">
+        <v>85.78364631652832</v>
+      </c>
+      <c r="L15" s="1">
+        <v>84.25482885742187</v>
+      </c>
+      <c r="M15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="2">
+        <v>-0.08</v>
+      </c>
+      <c r="P15">
+        <v>55.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>67135.578125</v>
+      </c>
+      <c r="J16" s="1">
+        <v>67809.8671875</v>
+      </c>
+      <c r="K16" s="1">
+        <v>67806.93390625001</v>
+      </c>
+      <c r="L16" s="1">
+        <v>66598.4935</v>
+      </c>
+      <c r="M16" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="P16">
+        <v>55.18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.2847498953342438</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.2812590003013611</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.2819023963809013</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.2870278944969177</v>
+      </c>
+      <c r="M17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="P17">
+        <v>55.26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1983.845458984375</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2004.282348632812</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2003.683913574219</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1967.9746953125</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P18">
+        <v>55.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="I19" s="1">
+        <v>614.979736328125</v>
+      </c>
+      <c r="J19" s="1">
+        <v>621.5844116210938</v>
+      </c>
+      <c r="K19" s="1">
+        <v>621.1295336914062</v>
+      </c>
+      <c r="L19" s="1">
+        <v>610.0598984375</v>
+      </c>
+      <c r="M19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="P19">
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2.22</v>
+      </c>
+      <c r="I20" s="1">
+        <v>68299.15625</v>
+      </c>
+      <c r="J20" s="1">
+        <v>67500.203125</v>
+      </c>
+      <c r="K20" s="1">
+        <v>67616.1646875</v>
+      </c>
+      <c r="L20" s="1">
+        <v>68845.54949999999</v>
+      </c>
+      <c r="M20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="P20">
+        <v>55.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2.22</v>
+      </c>
+      <c r="I21" s="1">
+        <v>67285.1796875</v>
+      </c>
+      <c r="J21" s="1">
+        <v>68226.15625</v>
+      </c>
+      <c r="K21" s="1">
+        <v>67958.03148437499</v>
+      </c>
+      <c r="L21" s="1">
+        <v>66746.89825</v>
+      </c>
+      <c r="M21" t="s">
+        <v>78</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="P21">
+        <v>55.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.22</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1951.21435546875</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1934.767578125</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1970.726499023438</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1935.604640625</v>
+      </c>
+      <c r="M22" t="s">
+        <v>79</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22" s="2">
+        <v>-0.06</v>
+      </c>
+      <c r="P22">
+        <v>55.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Relatório V164 Atualizado: Thu Feb 19 17:28:22 UTC 2026
</commit_message>
<xml_diff>
--- a/Relatorio_Oficial.xlsx
+++ b/Relatorio_Oficial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="67">
   <si>
     <t>Data</t>
   </si>
@@ -46,13 +46,175 @@
     <t>INICIO</t>
   </si>
   <si>
+    <t>18/02/2026 22:45:47</t>
+  </si>
+  <si>
+    <t>18/02/2026 22:48:52</t>
+  </si>
+  <si>
+    <t>18/02/2026 22:50:51</t>
+  </si>
+  <si>
+    <t>18/02/2026 22:52:58</t>
+  </si>
+  <si>
+    <t>18/02/2026 22:55:53</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:09:50</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:11:55</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:13:56</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:18:51</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:24:54</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:26:50</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:29:55</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:31:51</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:38:49</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:40:49</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:42:50</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:44:50</t>
+  </si>
+  <si>
+    <t>18/02/2026 23:46:53</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:01:52</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:18:49</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:34:55</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:36:53</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:38:51</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:40:51</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:42:54</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:44:47</t>
+  </si>
+  <si>
+    <t>19/02/2026 00:46:55</t>
+  </si>
+  <si>
+    <t>19/02/2026 01:01:54</t>
+  </si>
+  <si>
+    <t>19/02/2026 01:10:50</t>
+  </si>
+  <si>
+    <t>19/02/2026 01:13:52</t>
+  </si>
+  <si>
+    <t>19/02/2026 01:15:48</t>
+  </si>
+  <si>
+    <t>19/02/2026 01:17:54</t>
+  </si>
+  <si>
+    <t>19/02/2026 02:28:01</t>
+  </si>
+  <si>
+    <t>19/02/2026 02:38:46</t>
+  </si>
+  <si>
+    <t>19/02/2026 03:11:55</t>
+  </si>
+  <si>
+    <t>19/02/2026 03:13:47</t>
+  </si>
+  <si>
+    <t>19/02/2026 03:15:49</t>
+  </si>
+  <si>
+    <t>19/02/2026 04:20:48</t>
+  </si>
+  <si>
+    <t>19/02/2026 05:33:49</t>
+  </si>
+  <si>
+    <t>19/02/2026 06:12:51</t>
+  </si>
+  <si>
+    <t>19/02/2026 06:24:46</t>
+  </si>
+  <si>
+    <t>19/02/2026 11:50:55</t>
+  </si>
+  <si>
+    <t>19/02/2026 14:21:52</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
+    <t>BNB-USD</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
+  </si>
+  <si>
+    <t>ADA-USD</t>
+  </si>
+  <si>
+    <t>ETH-USD</t>
+  </si>
+  <si>
+    <t>SOL-USD</t>
+  </si>
+  <si>
     <t>Depósito</t>
   </si>
   <si>
+    <t>TREND</t>
+  </si>
+  <si>
+    <t>TRAP</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
     <t>Saldo Inicial</t>
+  </si>
+  <si>
+    <t>✅ TP Fast (EMA20)</t>
+  </si>
+  <si>
+    <t>✅ TP Trap</t>
+  </si>
+  <si>
+    <t>⛔ STOP LOSS</t>
   </si>
 </sst>
 </file>
@@ -197,23 +359,281 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Trades_V164!$A$2</c:f>
+              <c:f>Trades_V164!$A$2:$A$45</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>INICIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18/02/2026 22:45:47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18/02/2026 22:48:52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18/02/2026 22:50:51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18/02/2026 22:52:58</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18/02/2026 22:55:53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18/02/2026 23:09:50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18/02/2026 23:11:55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18/02/2026 23:13:56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18/02/2026 23:18:51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18/02/2026 23:24:54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18/02/2026 23:26:50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18/02/2026 23:29:55</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18/02/2026 23:31:51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18/02/2026 23:38:49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18/02/2026 23:40:49</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18/02/2026 23:42:50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18/02/2026 23:44:50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18/02/2026 23:46:53</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19/02/2026 00:01:52</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19/02/2026 00:18:49</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19/02/2026 00:34:55</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19/02/2026 00:36:53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19/02/2026 00:38:51</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19/02/2026 00:40:51</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>19/02/2026 00:42:54</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19/02/2026 00:44:47</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19/02/2026 00:46:55</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19/02/2026 01:01:54</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19/02/2026 01:10:50</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19/02/2026 01:13:52</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19/02/2026 01:15:48</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19/02/2026 01:17:54</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19/02/2026 02:28:01</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>19/02/2026 02:38:46</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19/02/2026 03:11:55</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>19/02/2026 03:13:47</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19/02/2026 03:15:49</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19/02/2026 04:20:48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19/02/2026 05:33:49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19/02/2026 06:12:51</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19/02/2026 06:24:46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19/02/2026 11:50:55</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19/02/2026 14:21:52</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Trades_V164!$I$2</c:f>
+              <c:f>Trades_V164!$I$2:$I$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59.99</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60.00000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>59.99000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>60.00000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>60.00000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>60.01000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>59.96000000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60.02000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60.01000000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60.00000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>60.07000000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>59.98000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -584,7 +1004,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,28 +1051,1275 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
       </c>
       <c r="I2" s="2">
         <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I3" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>59.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I16" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I21" s="2">
+        <v>60.00000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I22" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>59.99000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I35" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I36" s="2">
+        <v>60.00000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>60.00000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="I38" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" s="2">
+        <v>-0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>60.01000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="I40" s="2">
+        <v>59.96000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="I41" s="2">
+        <v>60.02000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I42" s="2">
+        <v>60.01000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="I43" s="2">
+        <v>60.00000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I44" s="2">
+        <v>60.07000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" s="2">
+        <v>-0.09</v>
+      </c>
+      <c r="I45" s="2">
+        <v>59.98000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>